<commit_message>
Minor fix in PS bit index
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2024_v1_1_0/PrescaleTable/L1Menu_Collisions2024_v1_1_0.xlsx
+++ b/official/L1Menu_Collisions2024_v1_1_0/PrescaleTable/L1Menu_Collisions2024_v1_1_0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2024_v1_1_0/PStables_official/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-master 25/official/L1Menu_Collisions2024_v1_1_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B3E7A6-308A-104D-979E-825D0EDE96FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F493BB-776D-054C-99E2-2851FE71B1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="B196" sqref="B196"/>
+    <sheetView tabSelected="1" topLeftCell="A309" workbookViewId="0">
+      <selection activeCell="A340" sqref="A340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15467,7 +15467,7 @@
     </row>
     <row r="338" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A338">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B338" s="6" t="s">
         <v>397</v>
@@ -15508,7 +15508,7 @@
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A339">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B339" s="6" t="s">
         <v>398</v>

</xml_diff>